<commit_message>
Updated to have cooling in non-residential use types
</commit_message>
<xml_diff>
--- a/remap_ville_plugin/CH_ReMaP/archetypes/CONSTRUCTION_STANDARD_SUMMARY.xlsx
+++ b/remap_ville_plugin/CH_ReMaP/archetypes/CONSTRUCTION_STANDARD_SUMMARY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aoraiopoulos\Documents\GitHub\cea-remap-ville-plugin\remap_ville_plugin\CH_ReMaP\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E25C40-6A76-448A-B0B7-D2EC95059DEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D55EDC7-80A8-42B9-9F25-3557C5856A3C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="4065" windowWidth="38640" windowHeight="21240" tabRatio="785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="4065" windowWidth="38640" windowHeight="21240" tabRatio="785" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STANDARD_DEFINITION" sheetId="10" r:id="rId1"/>
@@ -1528,7 +1528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
@@ -5612,11 +5612,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F44" sqref="F44:F55"/>
+      <selection pane="bottomRight" activeCell="C44" sqref="C44:C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6696,7 +6696,7 @@
         <v>50</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>145</v>
@@ -6728,7 +6728,7 @@
         <v>50</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>51</v>
+        <v>147</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>145</v>
@@ -6760,7 +6760,7 @@
         <v>50</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>145</v>
@@ -6792,7 +6792,7 @@
         <v>50</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>51</v>
+        <v>147</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>145</v>
@@ -6824,7 +6824,7 @@
         <v>50</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>145</v>
@@ -6856,7 +6856,7 @@
         <v>50</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>51</v>
+        <v>147</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>145</v>
@@ -6888,7 +6888,7 @@
         <v>50</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>145</v>
@@ -6920,7 +6920,7 @@
         <v>50</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>51</v>
+        <v>147</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>145</v>
@@ -6952,7 +6952,7 @@
         <v>50</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>145</v>
@@ -6984,7 +6984,7 @@
         <v>50</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>51</v>
+        <v>147</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>145</v>
@@ -7404,7 +7404,7 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D46" sqref="D46:D55"/>
+      <selection activeCell="A32" sqref="A32:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7944,7 +7944,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="2" t="s">
         <v>173</v>
       </c>
@@ -8359,6 +8359,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4119BA2A2C9A34A9ABDCD539C093B2A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2036187cb88b360b5a6de576d0a5f2f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="be70d004-d1e5-4317-a402-eff109a4a2bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e63961df46f11abd186e13992df6f3c7" ns3:_="">
     <xsd:import namespace="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
@@ -8528,12 +8534,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -8544,6 +8544,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8561,22 +8577,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Updated No Cooling for UC and F for Residential
</commit_message>
<xml_diff>
--- a/remap_ville_plugin/CH_ReMaP/archetypes/CONSTRUCTION_STANDARD_SUMMARY.xlsx
+++ b/remap_ville_plugin/CH_ReMaP/archetypes/CONSTRUCTION_STANDARD_SUMMARY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aoraiopoulos\Documents\GitHub\cea-remap-ville-plugin\remap_ville_plugin\CH_ReMaP\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D55EDC7-80A8-42B9-9F25-3557C5856A3C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C36846-6E35-4365-97FA-33778A2365A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="4065" windowWidth="38640" windowHeight="21240" tabRatio="785" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3600" yWindow="2415" windowWidth="21600" windowHeight="12495" tabRatio="785" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STANDARD_DEFINITION" sheetId="10" r:id="rId1"/>
@@ -1532,15 +1532,15 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.26171875" customWidth="1"/>
-    <col min="2" max="2" width="70.26171875" customWidth="1"/>
-    <col min="3" max="3" width="11.83984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.15625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="70.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>149</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>150</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>151</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>152</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>153</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>154</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>155</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>156</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>157</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>158</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>159</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>160</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>161</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>162</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>163</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>164</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>165</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>166</v>
       </c>
@@ -1890,7 +1890,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>167</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>168</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>169</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>170</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>171</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>172</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>173</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>174</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>175</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>176</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>177</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>178</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>179</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>180</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>181</v>
       </c>
@@ -2100,7 +2100,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>182</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>183</v>
       </c>
@@ -2128,7 +2128,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>184</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>185</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>186</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>187</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>188</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>1970</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>189</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>190</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>1980</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>191</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>192</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>193</v>
       </c>
@@ -2268,7 +2268,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>194</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>195</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>196</v>
       </c>
@@ -2330,29 +2330,29 @@
       <selection pane="bottomRight" activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.83984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.26171875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11" style="1" customWidth="1"/>
-    <col min="8" max="9" width="11.83984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.15625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.26171875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.68359375" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.83984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.15625" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.15625" style="1"/>
+    <col min="16" max="16" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="T2" s="6"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -2531,7 +2531,7 @@
       </c>
       <c r="T3" s="6"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -2591,7 +2591,7 @@
       </c>
       <c r="T4" s="6"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -2651,7 +2651,7 @@
       </c>
       <c r="T5" s="6"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>149</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>150</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>151</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>152</v>
       </c>
@@ -3005,7 +3005,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>153</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>154</v>
       </c>
@@ -3123,7 +3123,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>155</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>156</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>157</v>
       </c>
@@ -3300,7 +3300,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>158</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>159</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>160</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>161</v>
       </c>
@@ -3536,7 +3536,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>162</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>163</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>164</v>
       </c>
@@ -3713,7 +3713,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>165</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>166</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>167</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>168</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>169</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>170</v>
       </c>
@@ -4067,7 +4067,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>171</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>172</v>
       </c>
@@ -4185,7 +4185,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>173</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>174</v>
       </c>
@@ -4303,7 +4303,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>175</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>176</v>
       </c>
@@ -4421,7 +4421,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>177</v>
       </c>
@@ -4480,7 +4480,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>178</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>179</v>
       </c>
@@ -4598,7 +4598,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>180</v>
       </c>
@@ -4657,7 +4657,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>181</v>
       </c>
@@ -4716,7 +4716,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>182</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>183</v>
       </c>
@@ -4834,7 +4834,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>184</v>
       </c>
@@ -4893,7 +4893,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>185</v>
       </c>
@@ -4952,7 +4952,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>186</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>187</v>
       </c>
@@ -5070,7 +5070,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>188</v>
       </c>
@@ -5129,7 +5129,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>189</v>
       </c>
@@ -5188,7 +5188,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>190</v>
       </c>
@@ -5247,7 +5247,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>191</v>
       </c>
@@ -5306,7 +5306,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>192</v>
       </c>
@@ -5365,7 +5365,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>193</v>
       </c>
@@ -5424,7 +5424,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>194</v>
       </c>
@@ -5483,7 +5483,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>195</v>
       </c>
@@ -5542,7 +5542,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>196</v>
       </c>
@@ -5613,26 +5613,26 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C44" sqref="C44:C55"/>
+      <selection pane="bottomRight" activeCell="A45" sqref="A45:XFD45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.41796875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="19.41796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="21.68359375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.15625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.26171875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.15625" style="1"/>
+    <col min="1" max="1" width="15.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -5664,7 +5664,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -5728,7 +5728,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -5760,7 +5760,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -5792,7 +5792,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -5824,7 +5824,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -5856,7 +5856,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>149</v>
       </c>
@@ -5888,7 +5888,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>150</v>
       </c>
@@ -5920,7 +5920,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>151</v>
       </c>
@@ -5952,7 +5952,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>152</v>
       </c>
@@ -5984,7 +5984,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>153</v>
       </c>
@@ -6016,7 +6016,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>154</v>
       </c>
@@ -6048,7 +6048,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>155</v>
       </c>
@@ -6080,7 +6080,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>156</v>
       </c>
@@ -6112,7 +6112,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>157</v>
       </c>
@@ -6144,7 +6144,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>158</v>
       </c>
@@ -6176,7 +6176,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>159</v>
       </c>
@@ -6208,7 +6208,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>160</v>
       </c>
@@ -6240,7 +6240,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>161</v>
       </c>
@@ -6272,7 +6272,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>162</v>
       </c>
@@ -6304,7 +6304,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>163</v>
       </c>
@@ -6336,7 +6336,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>164</v>
       </c>
@@ -6368,7 +6368,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>165</v>
       </c>
@@ -6400,7 +6400,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>166</v>
       </c>
@@ -6432,7 +6432,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>167</v>
       </c>
@@ -6464,7 +6464,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>168</v>
       </c>
@@ -6496,7 +6496,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>169</v>
       </c>
@@ -6528,7 +6528,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>170</v>
       </c>
@@ -6560,7 +6560,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>171</v>
       </c>
@@ -6592,7 +6592,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>172</v>
       </c>
@@ -6624,7 +6624,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>173</v>
       </c>
@@ -6656,7 +6656,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>174</v>
       </c>
@@ -6688,7 +6688,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>175</v>
       </c>
@@ -6696,7 +6696,7 @@
         <v>50</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>146</v>
+        <v>51</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>145</v>
@@ -6720,7 +6720,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>176</v>
       </c>
@@ -6752,7 +6752,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>177</v>
       </c>
@@ -6760,7 +6760,7 @@
         <v>50</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>146</v>
+        <v>51</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>145</v>
@@ -6784,7 +6784,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>178</v>
       </c>
@@ -6816,7 +6816,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>179</v>
       </c>
@@ -6824,7 +6824,7 @@
         <v>50</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>146</v>
+        <v>51</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>145</v>
@@ -6848,7 +6848,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>180</v>
       </c>
@@ -6880,7 +6880,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>181</v>
       </c>
@@ -6888,7 +6888,7 @@
         <v>50</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>146</v>
+        <v>51</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>145</v>
@@ -6912,7 +6912,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>182</v>
       </c>
@@ -6944,7 +6944,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>183</v>
       </c>
@@ -6952,7 +6952,7 @@
         <v>50</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>146</v>
+        <v>51</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>145</v>
@@ -6976,7 +6976,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>184</v>
       </c>
@@ -7008,7 +7008,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>185</v>
       </c>
@@ -7040,7 +7040,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>186</v>
       </c>
@@ -7072,7 +7072,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>187</v>
       </c>
@@ -7080,7 +7080,7 @@
         <v>50</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>146</v>
+        <v>51</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>145</v>
@@ -7104,7 +7104,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>188</v>
       </c>
@@ -7136,7 +7136,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>189</v>
       </c>
@@ -7144,7 +7144,7 @@
         <v>50</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>146</v>
+        <v>51</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>145</v>
@@ -7168,7 +7168,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>190</v>
       </c>
@@ -7200,7 +7200,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>191</v>
       </c>
@@ -7208,7 +7208,7 @@
         <v>50</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>146</v>
+        <v>51</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>145</v>
@@ -7232,7 +7232,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>192</v>
       </c>
@@ -7264,7 +7264,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>193</v>
       </c>
@@ -7272,7 +7272,7 @@
         <v>50</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>146</v>
+        <v>51</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>145</v>
@@ -7296,7 +7296,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>194</v>
       </c>
@@ -7328,7 +7328,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>195</v>
       </c>
@@ -7336,7 +7336,7 @@
         <v>50</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>146</v>
+        <v>51</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>145</v>
@@ -7360,7 +7360,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>196</v>
       </c>
@@ -7403,21 +7403,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD43"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.15625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="20.83984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.15625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.15625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.15625" style="1"/>
+    <col min="1" max="1" width="15.140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
@@ -7434,7 +7434,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -7451,7 +7451,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>32</v>
       </c>
@@ -7468,7 +7468,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -7485,7 +7485,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
@@ -7502,7 +7502,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -7519,7 +7519,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>36</v>
       </c>
@@ -7536,7 +7536,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>149</v>
       </c>
@@ -7553,7 +7553,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>150</v>
       </c>
@@ -7570,7 +7570,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>151</v>
       </c>
@@ -7587,7 +7587,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>152</v>
       </c>
@@ -7604,7 +7604,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>153</v>
       </c>
@@ -7621,7 +7621,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>154</v>
       </c>
@@ -7638,7 +7638,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>155</v>
       </c>
@@ -7655,7 +7655,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>156</v>
       </c>
@@ -7672,7 +7672,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>157</v>
       </c>
@@ -7689,7 +7689,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>158</v>
       </c>
@@ -7706,7 +7706,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>159</v>
       </c>
@@ -7723,7 +7723,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>160</v>
       </c>
@@ -7740,7 +7740,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>161</v>
       </c>
@@ -7757,7 +7757,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>162</v>
       </c>
@@ -7774,7 +7774,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>163</v>
       </c>
@@ -7791,7 +7791,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>164</v>
       </c>
@@ -7808,7 +7808,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>165</v>
       </c>
@@ -7825,7 +7825,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>166</v>
       </c>
@@ -7842,7 +7842,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>167</v>
       </c>
@@ -7859,7 +7859,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>168</v>
       </c>
@@ -7876,7 +7876,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>169</v>
       </c>
@@ -7893,7 +7893,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>170</v>
       </c>
@@ -7910,7 +7910,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>171</v>
       </c>
@@ -7927,7 +7927,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>172</v>
       </c>
@@ -7944,7 +7944,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>173</v>
       </c>
@@ -7961,7 +7961,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>174</v>
       </c>
@@ -7978,7 +7978,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>175</v>
       </c>
@@ -7989,13 +7989,13 @@
         <v>199</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>201</v>
+        <v>59</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>176</v>
       </c>
@@ -8012,7 +8012,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>177</v>
       </c>
@@ -8023,13 +8023,13 @@
         <v>199</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>201</v>
+        <v>59</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>178</v>
       </c>
@@ -8046,7 +8046,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>179</v>
       </c>
@@ -8057,13 +8057,13 @@
         <v>199</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>201</v>
+        <v>59</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>180</v>
       </c>
@@ -8080,7 +8080,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>181</v>
       </c>
@@ -8091,13 +8091,13 @@
         <v>199</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>201</v>
+        <v>59</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>182</v>
       </c>
@@ -8114,7 +8114,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>183</v>
       </c>
@@ -8125,13 +8125,13 @@
         <v>200</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>202</v>
+        <v>59</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>184</v>
       </c>
@@ -8148,7 +8148,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>185</v>
       </c>
@@ -8165,7 +8165,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>186</v>
       </c>
@@ -8182,7 +8182,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>187</v>
       </c>
@@ -8193,13 +8193,13 @@
         <v>199</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>201</v>
+        <v>59</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>188</v>
       </c>
@@ -8216,7 +8216,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>189</v>
       </c>
@@ -8227,13 +8227,13 @@
         <v>199</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>201</v>
+        <v>59</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>190</v>
       </c>
@@ -8250,7 +8250,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>191</v>
       </c>
@@ -8261,13 +8261,13 @@
         <v>199</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>201</v>
+        <v>59</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>192</v>
       </c>
@@ -8284,7 +8284,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>193</v>
       </c>
@@ -8295,13 +8295,13 @@
         <v>199</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>201</v>
+        <v>59</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>194</v>
       </c>
@@ -8318,7 +8318,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>195</v>
       </c>
@@ -8329,13 +8329,13 @@
         <v>200</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>202</v>
+        <v>59</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>196</v>
       </c>
@@ -8365,6 +8365,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4119BA2A2C9A34A9ABDCD539C093B2A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2036187cb88b360b5a6de576d0a5f2f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="be70d004-d1e5-4317-a402-eff109a4a2bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e63961df46f11abd186e13992df6f3c7" ns3:_="">
     <xsd:import namespace="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
@@ -8534,15 +8543,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
   <ds:schemaRefs>
@@ -8560,6 +8560,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8575,12 +8583,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>